<commit_message>
Add name on account to tokenized bank accounts
</commit_message>
<xml_diff>
--- a/templates/Tokenized Bank Accounts.xlsx
+++ b/templates/Tokenized Bank Accounts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -33,8 +33,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Some payment processors create a customer profile when tokenizing cards. If your payment processor does this, add the profile identifier here.</t>
+          <t xml:space="preserve">Some payment processors create a customer profile when tokenizing cards. If your payment processor does this, add the profile identifier here.</t>
         </r>
       </text>
     </comment>
@@ -45,8 +46,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>The tokenized eCheck number</t>
+          <t xml:space="preserve">The tokenized eCheck number</t>
         </r>
       </text>
     </comment>
@@ -57,8 +59,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>The last few digits of the bank account number</t>
+          <t xml:space="preserve">The last few digits of the bank account number</t>
         </r>
       </text>
     </comment>
@@ -69,8 +72,22 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>1 if this method should be used for auto pay, 0 if not.</t>
+          <t xml:space="preserve">1 if this method should be used for auto pay, 0 if not.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The name on the bank account</t>
         </r>
       </text>
     </comment>
@@ -79,21 +96,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Account ID</t>
-  </si>
-  <si>
-    <t>Payment Processor Customer Profile ID</t>
-  </si>
-  <si>
-    <t>Token</t>
-  </si>
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>Auto</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">Account ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment Processor Customer Profile ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name on Account</t>
   </si>
 </sst>
 </file>
@@ -101,13 +121,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -127,23 +148,11 @@
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -212,7 +221,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,19 +308,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>782640</xdr:colOff>
+      <xdr:colOff>782280</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="39960" y="19080"/>
-          <a:ext cx="7245000" cy="5010480"/>
+          <a:ext cx="7244640" cy="5010120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -323,28 +332,80 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0"/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>Use this sheet to import previously tokenized eCheck accounts. Make sure you have configured your eCheck processor in Sonar before proceeding.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>Grey columns are required, blue columns are optional.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -360,18 +421,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -385,17 +446,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.18"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -414,11 +477,14 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>